<commit_message>
progress in cohorts made
</commit_message>
<xml_diff>
--- a/schemas/individuals.xlsx
+++ b/schemas/individuals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oriol/Desktop/beacon-ri-tools-v2/schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D420D3-EC62-F041-A741-EF44122D937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD5F39-B06B-5C45-BB21-8C10B27FEF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="20480" windowHeight="16280" xr2:uid="{87B92365-A1C0-5249-B08E-5FDC9D9FECD5}"/>
+    <workbookView xWindow="1040" yWindow="620" windowWidth="20480" windowHeight="16280" xr2:uid="{87B92365-A1C0-5249-B08E-5FDC9D9FECD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
   <si>
     <t>diseases_ageOfOnset_iso8601duration</t>
   </si>
@@ -421,25 +421,10 @@
     <t>OPCS(v4-0.0):Ligation of visceral branch of abdominal aorta NEC</t>
   </si>
   <si>
-    <t>LOINC:35925-4</t>
-  </si>
-  <si>
-    <t>BMI</t>
-  </si>
-  <si>
-    <t>NCIT:C49671</t>
-  </si>
-  <si>
-    <t>Kilogram per Square Meter</t>
-  </si>
-  <si>
     <t>NCIT:C20197</t>
   </si>
   <si>
     <t>male</t>
-  </si>
-  <si>
-    <t>24-9-2021</t>
   </si>
   <si>
     <t>pedigrees_disease_ageOfOnset</t>
@@ -487,6 +472,24 @@
       </rPr>
       <t>fake1</t>
     </r>
+  </si>
+  <si>
+    <t>LOINC:35925-4,LOINC:3141-9</t>
+  </si>
+  <si>
+    <t>BMI,Weight</t>
+  </si>
+  <si>
+    <t>24-9-2021,24-9-2021</t>
+  </si>
+  <si>
+    <t>NCIT:C49671,NCIT:C28252</t>
+  </si>
+  <si>
+    <t>Kilogram per Square Meter,Kilogram</t>
+  </si>
+  <si>
+    <t>26.63838307,85.6358</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F7517F-4859-8048-B2B9-9ACB604AA4D2}">
   <dimension ref="A1:EF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
       <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
@@ -1108,7 +1111,7 @@
         <v>75</v>
       </c>
       <c r="BZ1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="CA1" t="s">
         <v>76</v>
@@ -1183,10 +1186,10 @@
         <v>98</v>
       </c>
       <c r="CZ1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="DA1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="DD1" t="s">
         <v>121</v>
@@ -1252,13 +1255,13 @@
         <v>118</v>
       </c>
       <c r="DY1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="DZ1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="EA1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="EE1" t="s">
         <v>119</v>
@@ -1278,7 +1281,7 @@
         <v>125</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>126</v>
@@ -1287,28 +1290,28 @@
         <v>127</v>
       </c>
       <c r="AT2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="DS2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="DT2" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BC2" s="3">
-        <v>26.63838307</v>
-      </c>
-      <c r="DS2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DT2" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>